<commit_message>
working on annotations and factory refactoring
</commit_message>
<xml_diff>
--- a/sbmlutils/dfba/toy_atp/annotations.xlsx
+++ b/sbmlutils/dfba/toy_atp/annotations.xlsx
@@ -31,13 +31,13 @@
     <t xml:space="preserve">annotation_type</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
     <t xml:space="preserve">qualifier</t>
   </si>
   <si>
     <t xml:space="preserve">collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -55,31 +55,31 @@
     <t xml:space="preserve">RDF</t>
   </si>
   <si>
-    <t xml:space="preserve">PW:0000640</t>
-  </si>
-  <si>
     <t xml:space="preserve">BQB_IS_VERSION_OF</t>
   </si>
   <si>
     <t xml:space="preserve">pw</t>
   </si>
   <si>
+    <t xml:space="preserve">PW:0000640</t>
+  </si>
+  <si>
     <t xml:space="preserve">glycolysis pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kegg.pathway</t>
   </si>
   <si>
     <t xml:space="preserve">map00010</t>
   </si>
   <si>
-    <t xml:space="preserve">kegg.pathway</t>
-  </si>
-  <si>
     <t xml:space="preserve">Glycolysis / gluconeogenesis</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0006007</t>
+    <t xml:space="preserve">go</t>
   </si>
   <si>
-    <t xml:space="preserve">go</t>
+    <t xml:space="preserve">GO:0006007</t>
   </si>
   <si>
     <t xml:space="preserve">glucose catabolic process</t>
@@ -94,13 +94,13 @@
     <t xml:space="preserve">unit</t>
   </si>
   <si>
-    <t xml:space="preserve">UO:0000032</t>
-  </si>
-  <si>
     <t xml:space="preserve">BQB_IS</t>
   </si>
   <si>
     <t xml:space="preserve">uo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UO:0000032</t>
   </si>
   <si>
     <t xml:space="preserve">hour</t>
@@ -160,10 +160,10 @@
     <t xml:space="preserve">compartment</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000290</t>
+    <t xml:space="preserve">sbo</t>
   </si>
   <si>
-    <t xml:space="preserve">biomodels.sbo</t>
+    <t xml:space="preserve">SBO:0000290</t>
   </si>
   <si>
     <t xml:space="preserve">physical compartment</t>
@@ -172,10 +172,10 @@
     <t xml:space="preserve">GO:0005623</t>
   </si>
   <si>
-    <t xml:space="preserve">FMA:68646</t>
+    <t xml:space="preserve">fma</t>
   </si>
   <si>
-    <t xml:space="preserve">fma</t>
+    <t xml:space="preserve">FMA:68646</t>
   </si>
   <si>
     <t xml:space="preserve"># species</t>
@@ -193,19 +193,19 @@
     <t xml:space="preserve">simple chemical</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEBI:4167</t>
+    <t xml:space="preserve">chebi</t>
   </si>
   <si>
-    <t xml:space="preserve">chebi</t>
+    <t xml:space="preserve">CHEBI:4167</t>
   </si>
   <si>
     <t xml:space="preserve">D-glucopyranose</t>
   </si>
   <si>
-    <t xml:space="preserve">C00031</t>
+    <t xml:space="preserve">kegg.compound</t>
   </si>
   <si>
-    <t xml:space="preserve">kegg.compound</t>
+    <t xml:space="preserve">C00031</t>
   </si>
   <si>
     <t xml:space="preserve">D-Glucose</t>
@@ -515,12 +515,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -642,20 +642,21 @@
   </sheetPr>
   <dimension ref="1:71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G71" activeCellId="0" sqref="G71"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17 E22 E28 E34 E40 E46 E52 E59:E60 E63 E66 E70:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="12.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.219387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="35.2040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="12.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,13 +669,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -687,9 +688,9 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,13 +706,13 @@
       <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -726,15 +727,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -749,15 +750,15 @@
         <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -765,10 +766,10 @@
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -776,9 +777,9 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,16 +792,16 @@
       <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -814,16 +815,16 @@
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>29</v>
+      <c r="D9" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -837,16 +838,16 @@
       <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>32</v>
+      <c r="D10" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="F10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -860,16 +861,16 @@
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>35</v>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -883,16 +884,16 @@
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>38</v>
+      <c r="D12" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -906,16 +907,16 @@
       <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>41</v>
+      <c r="D13" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -923,19 +924,19 @@
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
@@ -943,9 +944,9 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,16 +959,16 @@
       <c r="C17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -981,16 +982,16 @@
       <c r="C18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1004,16 +1005,16 @@
       <c r="C19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1023,11 +1024,10 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
@@ -2055,19 +2055,18 @@
       <c r="C22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -3095,19 +3094,18 @@
       <c r="C23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -4135,19 +4133,18 @@
       <c r="C24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -5175,12 +5172,11 @@
       <c r="C25" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
@@ -6208,12 +6204,11 @@
       <c r="C26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="H26" s="0"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
@@ -7239,7 +7234,6 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-      <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
@@ -8267,14 +8261,14 @@
       <c r="C28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>56</v>
@@ -8290,14 +8284,14 @@
       <c r="C29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>69</v>
@@ -8313,14 +8307,14 @@
       <c r="C30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="14" t="s">
         <v>70</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>71</v>
@@ -8336,11 +8330,11 @@
       <c r="C31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
       <c r="G31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8353,11 +8347,11 @@
       <c r="C32" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
       <c r="G32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8379,14 +8373,14 @@
       <c r="C34" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>56</v>
@@ -8402,18 +8396,19 @@
       <c r="C35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>74</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>75</v>
       </c>
+      <c r="H35" s="0"/>
     </row>
     <row r="36" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
@@ -8425,18 +8420,19 @@
       <c r="C36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>77</v>
       </c>
+      <c r="H36" s="0"/>
     </row>
     <row r="37" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
@@ -8448,10 +8444,11 @@
       <c r="C37" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="E37" s="12"/>
+      <c r="F37" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="12"/>
+      <c r="H37" s="0"/>
     </row>
     <row r="38" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
@@ -8463,11 +8460,12 @@
       <c r="C38" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="H38" s="0"/>
     </row>
     <row r="39" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
@@ -8477,6 +8475,7 @@
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
+      <c r="H39" s="0"/>
     </row>
     <row r="40" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
@@ -8488,18 +8487,19 @@
       <c r="C40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="H40" s="0"/>
     </row>
     <row r="41" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
@@ -8511,18 +8511,19 @@
       <c r="C41" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>81</v>
       </c>
+      <c r="H41" s="0"/>
     </row>
     <row r="42" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
@@ -8534,18 +8535,19 @@
       <c r="C42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="H42" s="0"/>
     </row>
     <row r="43" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
@@ -8557,11 +8559,12 @@
       <c r="C43" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="H43" s="0"/>
     </row>
     <row r="44" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
@@ -8573,11 +8576,12 @@
       <c r="C44" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="H44" s="0"/>
     </row>
     <row r="45" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11"/>
@@ -8587,6 +8591,7 @@
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
+      <c r="H45" s="0"/>
     </row>
     <row r="46" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
@@ -8598,18 +8603,19 @@
       <c r="C46" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="H46" s="0"/>
     </row>
     <row r="47" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
@@ -8621,18 +8627,19 @@
       <c r="C47" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>87</v>
       </c>
+      <c r="H47" s="0"/>
     </row>
     <row r="48" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
@@ -8644,18 +8651,19 @@
       <c r="C48" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="14" t="s">
         <v>88</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>89</v>
       </c>
+      <c r="H48" s="0"/>
     </row>
     <row r="49" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
@@ -8667,11 +8675,12 @@
       <c r="C49" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
+      <c r="H49" s="0"/>
     </row>
     <row r="50" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
@@ -8683,11 +8692,12 @@
       <c r="C50" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="H50" s="0"/>
     </row>
     <row r="51" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11"/>
@@ -8697,6 +8707,7 @@
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
+      <c r="H51" s="0"/>
     </row>
     <row r="52" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="s">
@@ -8708,18 +8719,19 @@
       <c r="C52" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="H52" s="0"/>
     </row>
     <row r="53" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
@@ -8731,18 +8743,19 @@
       <c r="C53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>58</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>94</v>
       </c>
+      <c r="H53" s="0"/>
     </row>
     <row r="54" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
@@ -8754,18 +8767,19 @@
       <c r="C54" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>96</v>
       </c>
+      <c r="H54" s="0"/>
     </row>
     <row r="55" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
@@ -8777,11 +8791,12 @@
       <c r="C55" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="H55" s="0"/>
     </row>
     <row r="56" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
@@ -8793,20 +8808,22 @@
       <c r="C56" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="17" t="n">
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="17" t="n">
         <v>-3</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="H56" s="0"/>
     </row>
     <row r="57" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
-      <c r="D57" s="18"/>
+      <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
+      <c r="F57" s="18"/>
       <c r="G57" s="1"/>
+      <c r="H57" s="0"/>
     </row>
     <row r="58" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
@@ -8814,10 +8831,11 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="F58" s="6"/>
       <c r="G58" s="5"/>
+      <c r="H58" s="0"/>
     </row>
     <row r="59" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
@@ -8826,21 +8844,22 @@
       <c r="B59" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="9" t="s">
         <v>102</v>
       </c>
+      <c r="H59" s="0"/>
     </row>
     <row r="60" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
@@ -8852,27 +8871,29 @@
       <c r="C60" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E60" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" s="9" t="s">
         <v>105</v>
       </c>
+      <c r="H60" s="0"/>
     </row>
     <row r="61" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
+      <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="8"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="0"/>
     </row>
     <row r="62" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
@@ -8880,10 +8901,11 @@
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="F62" s="6"/>
       <c r="G62" s="5"/>
+      <c r="H62" s="0"/>
     </row>
     <row r="63" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
@@ -8895,18 +8917,19 @@
       <c r="C63" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="H63" s="0"/>
     </row>
     <row r="64" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
@@ -8919,17 +8942,18 @@
         <v>10</v>
       </c>
       <c r="D64" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G64" s="8" t="s">
+      <c r="G64" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="H64" s="0"/>
     </row>
     <row r="65" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
@@ -8937,8 +8961,9 @@
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="0"/>
     </row>
     <row r="66" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
@@ -8950,18 +8975,19 @@
       <c r="C66" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G66" s="9" t="s">
+      <c r="G66" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="H66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
@@ -8973,14 +8999,14 @@
       <c r="C67" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D67" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G67" s="19" t="s">
         <v>113</v>
@@ -8992,11 +9018,10 @@
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
-      <c r="D69" s="6"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="F69" s="6"/>
       <c r="G69" s="5"/>
-      <c r="H69" s="0"/>
       <c r="I69" s="0"/>
       <c r="J69" s="0"/>
       <c r="K69" s="0"/>
@@ -10024,19 +10049,18 @@
       <c r="C70" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E70" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G70" s="8" t="s">
+      <c r="G70" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H70" s="0"/>
       <c r="I70" s="0"/>
       <c r="J70" s="0"/>
       <c r="K70" s="0"/>
@@ -11064,19 +11088,18 @@
       <c r="C71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="E71" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G71" s="8" t="s">
+      <c r="G71" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H71" s="0"/>
       <c r="I71" s="0"/>
       <c r="J71" s="0"/>
       <c r="K71" s="0"/>

</xml_diff>